<commit_message>
Updated wrong sources to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -208,9 +208,6 @@
     <t>https://uk.rs-online.com/web/p/pcb-headers/2518086/</t>
   </si>
   <si>
-    <t>https://uk.rs-online.com/web/p/pcb-headers/8632813/</t>
-  </si>
-  <si>
     <t>https://uk.rs-online.com/web/p/pcb-headers/6812991/</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t>https://uk.rs-online.com/web/p/pcb-sockets/2518187/</t>
   </si>
   <si>
-    <t>https://uk.rs-online.com/web/p/pcb-sockets/9033554/</t>
-  </si>
-  <si>
     <t>4320-01074-0</t>
   </si>
   <si>
@@ -443,6 +437,18 @@
   </si>
   <si>
     <t>B01GDN1T4S</t>
+  </si>
+  <si>
+    <t>RMG Switch</t>
+  </si>
+  <si>
+    <t>https://www.rmgsailwinch.com.au/rmg/products/RMGSwitch%252dStd.html</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-headers/6812994/</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-sockets/1613692/</t>
   </si>
 </sst>
 </file>
@@ -685,8 +691,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I25" totalsRowCount="1">
-  <autoFilter ref="A1:I24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I26" totalsRowCount="1">
+  <autoFilter ref="A1:I25"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Value"/>
@@ -697,7 +703,7 @@
     <tableColumn id="7" name="Price">
       <calculatedColumnFormula>F2*$M$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="4">
+    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="0">
       <calculatedColumnFormula>F2*C2</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[Total])</totalsRowFormula>
     </tableColumn>
@@ -708,8 +714,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I9" totalsRowCount="1" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A1:I8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I10" totalsRowCount="1" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A1:I9"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Value"/>
@@ -720,7 +726,7 @@
     <tableColumn id="7" name="Price" dataDxfId="12">
       <calculatedColumnFormula>F2*$L$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="1">
       <calculatedColumnFormula>F2*C2</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table5[Total])-H2</totalsRowFormula>
     </tableColumn>
@@ -739,11 +745,11 @@
     <tableColumn id="3" name="Quantity"/>
     <tableColumn id="4" name="Reference"/>
     <tableColumn id="5" name="Description"/>
-    <tableColumn id="6" name="Price exc VAT" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Price" dataDxfId="7" totalsRowDxfId="1">
+    <tableColumn id="6" name="Price exc VAT" dataDxfId="8" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Price" dataDxfId="7" totalsRowDxfId="3">
       <calculatedColumnFormula>F2*$L$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="0">
+    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="2">
       <calculatedColumnFormula>F2*C2</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table6[Total])</totalsRowFormula>
     </tableColumn>
@@ -1018,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,104 +1051,104 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2">
-        <f>'Card Component'!H26</f>
-        <v>38.634</v>
+        <f>'Card Component'!H27</f>
+        <v>81.0732</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2">
         <f>Table5[[#Totals],[Total]]</f>
         <v>32.816666666666691</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2">
         <f>Table6[[#Totals],[Total]]</f>
         <v>427.10999999999996</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2">
         <f>14.93/1.2</f>
         <v>12.441666666666666</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8" s="2">
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" s="2">
         <v>7.53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f>SUM(Table4[Price])</f>
-        <v>556.53233333333333</v>
+        <v>598.97153333333335</v>
       </c>
     </row>
   </sheetData>
@@ -1164,11 +1170,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2">
         <v>0.08</v>
@@ -1457,7 +1463,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11" s="2">
         <v>0.432</v>
@@ -1482,21 +1488,21 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" s="2">
-        <v>0.13300000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>0.15959999999999999</v>
+        <v>0.24</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
-        <v>0.26600000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1507,7 +1513,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="2">
         <v>0.2</v>
@@ -1521,7 +1527,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1532,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F14" s="2">
         <v>0.84199999999999997</v>
@@ -1546,7 +1552,7 @@
         <v>0.84199999999999997</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1557,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15" s="2">
         <v>0.27500000000000002</v>
@@ -1571,7 +1577,7 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1647,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2">
         <v>5.3999999999999999E-2</v>
@@ -1661,7 +1667,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1675,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F19" s="2">
         <v>0.1</v>
@@ -1689,7 +1695,7 @@
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1700,7 +1706,7 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F20" s="2">
         <v>0.317</v>
@@ -1714,7 +1720,7 @@
         <v>2.2189999999999999</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1725,21 +1731,21 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F21" s="2">
-        <v>0.56999999999999995</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
-        <v>0.68399999999999994</v>
+        <v>1.1232</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
-        <v>1.1399999999999999</v>
+        <v>1.8720000000000001</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1750,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F22" s="2">
         <v>0.69099999999999995</v>
@@ -1764,7 +1770,7 @@
         <v>0.69099999999999995</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1775,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F23" s="2">
         <v>0.41799999999999998</v>
@@ -1789,7 +1795,7 @@
         <v>0.41799999999999998</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1800,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F24" s="2">
         <v>1.778</v>
@@ -1814,19 +1820,41 @@
         <v>1.778</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f>F25*$M$1</f>
+        <v>41.4</v>
+      </c>
       <c r="H25" s="2">
-        <f>SUM(Table1[Total])</f>
-        <v>32.195</v>
+        <f>F25*C25</f>
+        <v>34.5</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H26" s="2">
+        <f>SUM(Table1[Total])</f>
+        <v>67.561000000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="2">
         <f>Table1[[#Totals],[Total]]*M1</f>
-        <v>38.634</v>
+        <v>81.0732</v>
       </c>
     </row>
   </sheetData>
@@ -1845,30 +1873,29 @@
     <hyperlink ref="I21" r:id="rId12"/>
     <hyperlink ref="I23" r:id="rId13"/>
     <hyperlink ref="I24" r:id="rId14"/>
-    <hyperlink ref="I22" r:id="rId15"/>
-    <hyperlink ref="I11" r:id="rId16"/>
-    <hyperlink ref="I12" r:id="rId17"/>
-    <hyperlink ref="I13" r:id="rId18"/>
-    <hyperlink ref="I14" r:id="rId19"/>
-    <hyperlink ref="I15" r:id="rId20"/>
-    <hyperlink ref="I18" r:id="rId21"/>
-    <hyperlink ref="I19" r:id="rId22"/>
+    <hyperlink ref="I11" r:id="rId15"/>
+    <hyperlink ref="I13" r:id="rId16"/>
+    <hyperlink ref="I14" r:id="rId17"/>
+    <hyperlink ref="I15" r:id="rId18"/>
+    <hyperlink ref="I18" r:id="rId19"/>
+    <hyperlink ref="I19" r:id="rId20"/>
+    <hyperlink ref="I22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,13 +1945,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2">
         <v>206.6</v>
@@ -1938,12 +1965,12 @@
         <v>206.6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1960,12 +1987,12 @@
         <v>24.991666666666667</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -1974,7 +2001,7 @@
         <v>9.6199999999999994E-2</v>
       </c>
       <c r="G4" s="2">
-        <f>F4*$L$1</f>
+        <f t="shared" ref="G4:G9" si="1">F4*$L$1</f>
         <v>0.11543999999999999</v>
       </c>
       <c r="H4" s="2">
@@ -1982,27 +2009,27 @@
         <v>1.9239999999999999</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F5" s="2">
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="G5" s="2">
-        <f>F5*$L$1</f>
+        <f t="shared" si="1"/>
         <v>8.0400000000000003E-3</v>
       </c>
       <c r="H5" s="2">
@@ -2010,12 +2037,12 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2024,7 +2051,7 @@
         <v>0.76400000000000001</v>
       </c>
       <c r="G6" s="2">
-        <f>F6*$L$1</f>
+        <f t="shared" si="1"/>
         <v>0.91679999999999995</v>
       </c>
       <c r="H6" s="2">
@@ -2032,15 +2059,15 @@
         <v>0.76400000000000001</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2049,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="2">
-        <f>F7*$L$1</f>
+        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
       <c r="H7" s="2">
@@ -2057,15 +2084,15 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2074,7 +2101,7 @@
         <v>3.07</v>
       </c>
       <c r="G8" s="2">
-        <f>F8*$L$1</f>
+        <f t="shared" si="1"/>
         <v>3.6839999999999997</v>
       </c>
       <c r="H8" s="2">
@@ -2082,26 +2109,38 @@
         <v>3.07</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H9" s="2">
+        <f>F9*C9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="2">
         <f>SUM(Table5[Total])-H2</f>
         <v>32.816666666666691</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H10" s="2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="2">
         <f>Table5[[#Totals],[Total]]*L1</f>
         <v>39.380000000000031</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H12" s="2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="2">
         <f>SUM(Table5[Total])-H3</f>
         <v>214.42500000000001</v>
       </c>
@@ -2127,7 +2166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -2177,16 +2216,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
         <v>110</v>
-      </c>
-      <c r="E2" t="s">
-        <v>112</v>
       </c>
       <c r="F2" s="2">
         <v>262.77999999999997</v>
@@ -2200,12 +2239,12 @@
         <v>262.77999999999997</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2222,18 +2261,18 @@
         <v>5.08</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F4" s="2">
         <v>14.27</v>
@@ -2247,18 +2286,18 @@
         <v>14.27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2">
         <v>91.5</v>
@@ -2272,12 +2311,12 @@
         <v>91.5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2294,18 +2333,18 @@
         <v>24.5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>134</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>136</v>
       </c>
       <c r="F7" s="2">
         <v>28.98</v>
@@ -2319,7 +2358,7 @@
         <v>28.98</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated BOM for new board and wrong products
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -229,12 +229,6 @@
     <t>215297-8</t>
   </si>
   <si>
-    <t>https://uk.rs-online.com/web/p/pcb-sockets/7022899/</t>
-  </si>
-  <si>
-    <t>803-87-004-10-012101</t>
-  </si>
-  <si>
     <t>https://uk.rs-online.com/web/p/pcb-sockets/6742369/</t>
   </si>
   <si>
@@ -449,6 +443,81 @@
   </si>
   <si>
     <t>https://uk.rs-online.com/web/p/pcb-sockets/1613692/</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-sockets/7022934/</t>
+  </si>
+  <si>
+    <t>803-87-004-10-001101</t>
+  </si>
+  <si>
+    <t>PHR-2</t>
+  </si>
+  <si>
+    <t>JST PHR-2</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-housings/8201466/</t>
+  </si>
+  <si>
+    <t>JST PHR-3</t>
+  </si>
+  <si>
+    <t>JST PHR-4</t>
+  </si>
+  <si>
+    <t>PHR-3</t>
+  </si>
+  <si>
+    <t>PHR-4</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-housings/8201475/</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-housings/8201478/</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>SR560</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/rectifier-schottky-diodes/9179120/</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>12k</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/through-hole-fixed-resistors/1251166/</t>
+  </si>
+  <si>
+    <t>LR1F20K</t>
+  </si>
+  <si>
+    <t>MRS25000C1202FCT00</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/through-hole-fixed-resistors/6832989/</t>
+  </si>
+  <si>
+    <t>JST Cable</t>
+  </si>
+  <si>
+    <t>SPH-26L-300</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/products/8201412/</t>
+  </si>
+  <si>
+    <t>HXT 4 Prebuilt</t>
+  </si>
+  <si>
+    <t>https://hobbyking.com/en_us/hxt-4mm-gold-connector-w-pre-installed-bullets-10pcs-set.html</t>
   </si>
 </sst>
 </file>
@@ -691,8 +760,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I26" totalsRowCount="1">
-  <autoFilter ref="A1:I25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I30" totalsRowCount="1">
+  <autoFilter ref="A1:I29"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Value"/>
@@ -726,7 +795,7 @@
     <tableColumn id="7" name="Price" dataDxfId="12">
       <calculatedColumnFormula>F2*$L$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="1">
+    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="4">
       <calculatedColumnFormula>F2*C2</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table5[Total])-H2</totalsRowFormula>
     </tableColumn>
@@ -737,19 +806,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:I8" totalsRowCount="1" headerRowDxfId="10" headerRowBorderDxfId="9">
-  <autoFilter ref="A1:I7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:I13" totalsRowCount="1" headerRowDxfId="10" headerRowBorderDxfId="9">
+  <autoFilter ref="A1:I12"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Quantity"/>
     <tableColumn id="4" name="Reference"/>
     <tableColumn id="5" name="Description"/>
-    <tableColumn id="6" name="Price exc VAT" dataDxfId="8" totalsRowDxfId="4"/>
-    <tableColumn id="7" name="Price" dataDxfId="7" totalsRowDxfId="3">
+    <tableColumn id="6" name="Price exc VAT" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="7" name="Price" dataDxfId="7" totalsRowDxfId="2">
       <calculatedColumnFormula>F2*$L$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="2">
+    <tableColumn id="8" name="Total" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="1">
       <calculatedColumnFormula>F2*C2</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table6[Total])</totalsRowFormula>
     </tableColumn>
@@ -1051,104 +1120,104 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2">
-        <f>'Card Component'!H27</f>
-        <v>81.0732</v>
+        <f>'Card Component'!H31</f>
+        <v>80.506799999999998</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2">
         <f>Table5[[#Totals],[Total]]</f>
         <v>32.816666666666691</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" s="2">
         <f>Table6[[#Totals],[Total]]</f>
-        <v>427.10999999999996</v>
+        <v>434.35799999999995</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2">
         <f>14.93/1.2</f>
         <v>12.441666666666666</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" s="2">
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C9" s="2">
         <v>7.53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f>SUM(Table4[Price])</f>
-        <v>598.97153333333335</v>
+        <v>605.65313333333336</v>
       </c>
     </row>
   </sheetData>
@@ -1170,11 +1239,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1254,7 @@
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="67.42578125" customWidth="1"/>
+    <col min="9" max="9" width="88.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1236,7 +1305,7 @@
       <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>0.111</v>
       </c>
       <c r="G2">
@@ -1264,16 +1333,16 @@
       <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="F3">
-        <v>0.06</v>
+      <c r="F3" s="2">
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G24" si="0">F3*$M$1</f>
-        <v>7.1999999999999995E-2</v>
+        <v>9.1199999999999989E-2</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3:H24" si="1">F3*C3</f>
-        <v>0.06</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>50</v>
@@ -1292,7 +1361,7 @@
       <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.29199999999999998</v>
       </c>
       <c r="G4">
@@ -1320,7 +1389,7 @@
       <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.28899999999999998</v>
       </c>
       <c r="G5">
@@ -1340,12 +1409,12 @@
         <v>42</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.38</v>
       </c>
       <c r="G6">
@@ -1354,7 +1423,7 @@
       </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
-        <v>0.76</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>46</v>
@@ -1370,7 +1439,7 @@
       <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.38</v>
       </c>
       <c r="G7">
@@ -1390,7 +1459,7 @@
         <v>44</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -1404,7 +1473,7 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
-        <v>1.52</v>
+        <v>0.76</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>47</v>
@@ -1438,7 +1507,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2">
         <v>0.08</v>
@@ -1460,10 +1529,10 @@
         <v>19</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="2">
         <v>0.432</v>
@@ -1474,7 +1543,7 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>1.728</v>
+        <v>1.296</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>56</v>
@@ -1488,7 +1557,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" s="2">
         <v>0.2</v>
@@ -1502,7 +1571,7 @@
         <v>0.4</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1513,7 +1582,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2">
         <v>0.2</v>
@@ -1535,10 +1604,10 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14" s="2">
         <v>0.84199999999999997</v>
@@ -1549,7 +1618,7 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>0.84199999999999997</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>60</v>
@@ -1563,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F15" s="2">
         <v>0.27500000000000002</v>
@@ -1653,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F18" s="2">
         <v>5.3999999999999999E-2</v>
@@ -1667,7 +1736,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1681,7 +1750,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F19" s="2">
         <v>0.1</v>
@@ -1695,7 +1764,7 @@
         <v>0.2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1706,7 +1775,7 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="2">
         <v>0.317</v>
@@ -1745,7 +1814,7 @@
         <v>1.8720000000000001</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,21 +1850,21 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="F23" s="2">
-        <v>0.41799999999999998</v>
+        <v>0.45</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>0.50159999999999993</v>
+        <v>0.54</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
-        <v>0.41799999999999998</v>
+        <v>0.45</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1806,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F24" s="2">
         <v>1.778</v>
@@ -1820,41 +1889,145 @@
         <v>1.778</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>149</v>
       </c>
       <c r="F25" s="2">
-        <v>34.5</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="G25" s="2">
         <f>F25*$M$1</f>
-        <v>41.4</v>
+        <v>8.879999999999999E-2</v>
       </c>
       <c r="H25" s="2">
         <f>F25*C25</f>
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G26" s="2">
+        <f>F26*$M$1</f>
+        <v>5.2799999999999993E-2</v>
+      </c>
+      <c r="H26" s="2">
+        <f>F26*C26</f>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f>F27*$M$1</f>
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="H27" s="2">
+        <f>F27*C27</f>
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
         <v>34.5</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H26" s="2">
+      <c r="G28" s="2">
+        <f>F28*$M$1</f>
+        <v>41.4</v>
+      </c>
+      <c r="H28" s="2">
+        <f>F28*C28</f>
+        <v>34.5</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <f>7.15/10</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="G29" s="2">
+        <f>F29*$M$1</f>
+        <v>0.8580000000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <f>F29*C29</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="2">
         <f>SUM(Table1[Total])</f>
-        <v>67.561000000000007</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H27" s="2">
+        <v>67.088999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="2">
         <f>Table1[[#Totals],[Total]]*M1</f>
-        <v>81.0732</v>
+        <v>80.506799999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1871,20 +2044,25 @@
     <hyperlink ref="I10" r:id="rId10"/>
     <hyperlink ref="I20" r:id="rId11"/>
     <hyperlink ref="I21" r:id="rId12"/>
-    <hyperlink ref="I23" r:id="rId13"/>
-    <hyperlink ref="I24" r:id="rId14"/>
-    <hyperlink ref="I11" r:id="rId15"/>
-    <hyperlink ref="I13" r:id="rId16"/>
-    <hyperlink ref="I14" r:id="rId17"/>
-    <hyperlink ref="I15" r:id="rId18"/>
-    <hyperlink ref="I18" r:id="rId19"/>
-    <hyperlink ref="I19" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
+    <hyperlink ref="I24" r:id="rId13"/>
+    <hyperlink ref="I11" r:id="rId14"/>
+    <hyperlink ref="I13" r:id="rId15"/>
+    <hyperlink ref="I14" r:id="rId16"/>
+    <hyperlink ref="I15" r:id="rId17"/>
+    <hyperlink ref="I18" r:id="rId18"/>
+    <hyperlink ref="I19" r:id="rId19"/>
+    <hyperlink ref="I22" r:id="rId20"/>
+    <hyperlink ref="I23" r:id="rId21"/>
+    <hyperlink ref="I12" r:id="rId22"/>
+    <hyperlink ref="I28" r:id="rId23"/>
+    <hyperlink ref="I25" r:id="rId24"/>
+    <hyperlink ref="I27" r:id="rId25"/>
+    <hyperlink ref="I29" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1945,13 +2123,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="2">
         <v>206.6</v>
@@ -1965,12 +2143,12 @@
         <v>206.6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1987,12 +2165,12 @@
         <v>24.991666666666667</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -2009,21 +2187,21 @@
         <v>1.9239999999999999</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2">
         <v>6.7000000000000002E-3</v>
@@ -2037,12 +2215,12 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2059,15 +2237,15 @@
         <v>0.76400000000000001</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2084,15 +2262,15 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2109,7 +2287,7 @@
         <v>3.07</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2138,7 +2316,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H13" s="2">
         <f>SUM(Table5[Total])-H3</f>
@@ -2164,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,16 +2394,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
         <v>108</v>
-      </c>
-      <c r="E2" t="s">
-        <v>110</v>
       </c>
       <c r="F2" s="2">
         <v>262.77999999999997</v>
@@ -2239,12 +2417,12 @@
         <v>262.77999999999997</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2261,18 +2439,18 @@
         <v>5.08</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F4" s="2">
         <v>14.27</v>
@@ -2286,18 +2464,18 @@
         <v>14.27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F5" s="2">
         <v>91.5</v>
@@ -2311,12 +2489,12 @@
         <v>91.5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2333,18 +2511,18 @@
         <v>24.5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>132</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
       </c>
       <c r="F7" s="2">
         <v>28.98</v>
@@ -2358,21 +2536,133 @@
         <v>28.98</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f>F8*$L$1</f>
+        <v>3.7199999999999997E-2</v>
+      </c>
       <c r="H8" s="2">
+        <f>F8*C8</f>
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f>F9*$L$1</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <f>F9*C9</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="G10" s="2">
+        <f>F10*$L$1</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <f>F10*C10</f>
+        <v>0.08</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G11" s="2">
+        <f>F11*$L$1</f>
+        <v>0.56040000000000001</v>
+      </c>
+      <c r="H11" s="2">
+        <f>F11*C11</f>
+        <v>7.0050000000000008</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <f>F12*$L$1</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <f>F12*C12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
         <f>SUM(Table6[Total])</f>
-        <v>427.10999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H9" s="2">
+        <v>434.35799999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="2">
         <f>Table6[[#Totals],[Total]]*L1</f>
-        <v>512.53199999999993</v>
+        <v>521.22959999999989</v>
       </c>
     </row>
   </sheetData>
@@ -2382,10 +2672,14 @@
     <hyperlink ref="I3" r:id="rId3"/>
     <hyperlink ref="I5" r:id="rId4"/>
     <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I8" r:id="rId6"/>
+    <hyperlink ref="I9" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="I11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>